<commit_message>
Training Works - Last Sprint
</commit_message>
<xml_diff>
--- a/Administration/Ethics/Survey.xlsx
+++ b/Administration/Ethics/Survey.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d83c6986f351680b/Documents/dissertation-project/Administration/Ethics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\OneDrive\Documents\dissertation-project\Administration\Ethics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61FC73C6-5979-4B56-9731-5B3D35D42821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{61FC73C6-5979-4B56-9731-5B3D35D42821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF5E5AB8-C10F-4870-8A16-5755173E533F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99177323-558F-429A-A0B1-BC8353F831C1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Strongly Agree</t>
   </si>
@@ -60,9 +60,6 @@
     <t>I felt confident using features of the application</t>
   </si>
   <si>
-    <t>I feel that other users would be interested in this application</t>
-  </si>
-  <si>
     <t>There have been times in my past where I would have found this application useful</t>
   </si>
   <si>
@@ -70,6 +67,15 @@
   </si>
   <si>
     <t>I would recommend this application to other users</t>
+  </si>
+  <si>
+    <t>I felt the system's design was inconsistent</t>
+  </si>
+  <si>
+    <t>I was happy with the outputs of the application (e.g. were the results of the application organised in a way that you expected/approved of?).</t>
+  </si>
+  <si>
+    <t>The information produced by this application is useful/valuable</t>
   </si>
 </sst>
 </file>
@@ -93,15 +99,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -109,27 +133,142 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CFCF5C-D53B-4374-A810-A00899151F45}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,115 +601,170 @@
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="10">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="10">
         <v>2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="10">
         <v>3</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="9">
         <v>4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="B4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="B6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="16" t="s">
         <v>7</v>
       </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>